<commit_message>
Report - Package Diagram and update Planning
add Package Diagram and comments
also adjust Time Planning and add Workspace Management
</commit_message>
<xml_diff>
--- a/Document/ProcessManagement.xlsx
+++ b/Document/ProcessManagement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\University\3rdYear\1stSemester\Java\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\University\3rdYear\1stSemester\Java\Project\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70ABC8D-DD9F-4A04-84C8-CDCA952244E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A32FC7D-51DA-4FD9-BD50-DDF5590DA297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{39304C3B-05DB-44F2-8DEE-1B66E97C1637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{39304C3B-05DB-44F2-8DEE-1B66E97C1637}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1_Task" sheetId="5" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Khuê, Trung</t>
   </si>
   <si>
-    <t>Report - Result</t>
-  </si>
-  <si>
     <t>Implementation - Patient System - Admin side</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Package diagram</t>
+  </si>
+  <si>
+    <t>Report - Implementation and Result</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
                     <c:v>Report - Analysis and Design</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Report - Result</c:v>
+                    <c:v>Report - Implementation and Result</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>Report redesignation</c:v>
@@ -405,28 +405,28 @@
                 <c:formatCode>dd/mm</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44501</c:v>
+                  <c:v>44500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44501</c:v>
+                  <c:v>44500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44501</c:v>
+                  <c:v>44500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44501</c:v>
+                  <c:v>44500</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44507</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44509</c:v>
+                  <c:v>44507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44511</c:v>
+                  <c:v>44510</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44511</c:v>
+                  <c:v>44510</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>44513</c:v>
@@ -523,7 +523,7 @@
                     <c:v>Report - Analysis and Design</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Report - Result</c:v>
+                    <c:v>Report - Implementation and Result</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>Report redesignation</c:v>
@@ -539,28 +539,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -670,7 +670,7 @@
                     <c:v>Report - Analysis and Design</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Report - Result</c:v>
+                    <c:v>Report - Implementation and Result</c:v>
                   </c:pt>
                   <c:pt idx="8">
                     <c:v>Report redesignation</c:v>
@@ -799,7 +799,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44514"/>
-          <c:min val="44501"/>
+          <c:min val="44500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1097,13 +1097,13 @@
                 <c:formatCode>dd/mm</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>44515</c:v>
+                  <c:v>44514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44515</c:v>
+                  <c:v>44514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44515</c:v>
+                  <c:v>44514</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44525</c:v>
@@ -1186,13 +1186,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1386,7 +1386,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44528"/>
-          <c:min val="44515"/>
+          <c:min val="44514"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1684,13 +1684,13 @@
                 <c:formatCode>dd/mm</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>44529</c:v>
+                  <c:v>44528</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44529</c:v>
+                  <c:v>44528</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44529</c:v>
+                  <c:v>44528</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44539</c:v>
@@ -1773,13 +1773,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1973,7 +1973,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44542"/>
-          <c:min val="44529"/>
+          <c:min val="44528"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2277,7 +2277,7 @@
                 <c:formatCode>dd/mm</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>44543</c:v>
+                  <c:v>44542</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>44549</c:v>
@@ -2375,7 +2375,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -2587,7 +2587,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44556"/>
-          <c:min val="44543"/>
+          <c:min val="44542"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5385,12 +5385,12 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.375" style="1" bestFit="1" customWidth="1"/>
@@ -5434,10 +5434,10 @@
       </c>
       <c r="D2" s="6">
         <f>F2-E2</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
-        <v>44501</v>
+        <v>44500</v>
       </c>
       <c r="F2" s="4">
         <v>44507</v>
@@ -5458,10 +5458,10 @@
       </c>
       <c r="D3" s="6">
         <f>F3-E3</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
-        <v>44501</v>
+        <v>44500</v>
       </c>
       <c r="F3" s="4">
         <v>44507</v>
@@ -5482,10 +5482,10 @@
       </c>
       <c r="D4" s="6">
         <f>F4-E4</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4">
-        <v>44501</v>
+        <v>44500</v>
       </c>
       <c r="F4" s="4">
         <v>44507</v>
@@ -5506,10 +5506,10 @@
       </c>
       <c r="D5" s="6">
         <f>F5-E5</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="4">
-        <v>44501</v>
+        <v>44500</v>
       </c>
       <c r="F5" s="4">
         <v>44507</v>
@@ -5530,13 +5530,13 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" ref="D6:D7" si="0">F6-E6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4">
         <v>44507</v>
       </c>
       <c r="F6" s="4">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -5554,13 +5554,13 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
-        <v>44509</v>
+        <v>44507</v>
       </c>
       <c r="F7" s="4">
-        <v>44511</v>
+        <v>44510</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -5578,10 +5578,10 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ref="D8:D9" si="1">F8-E8</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="4">
-        <v>44511</v>
+        <v>44510</v>
       </c>
       <c r="F8" s="4">
         <v>44514</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -5602,10 +5602,10 @@
       </c>
       <c r="D9" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="4">
-        <v>44511</v>
+        <v>44510</v>
       </c>
       <c r="F9" s="4">
         <v>44514</v>
@@ -5648,7 +5648,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5663,7 +5663,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -5713,10 +5713,10 @@
       </c>
       <c r="D2" s="6">
         <f>F2-E2</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4">
-        <v>44515</v>
+        <v>44514</v>
       </c>
       <c r="F2" s="4">
         <v>44528</v>
@@ -5727,7 +5727,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -5737,10 +5737,10 @@
       </c>
       <c r="D3" s="6">
         <f>F3-E3</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>44515</v>
+        <v>44514</v>
       </c>
       <c r="F3" s="4">
         <v>44528</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -5761,10 +5761,10 @@
       </c>
       <c r="D4" s="6">
         <f>F4-E4</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4">
-        <v>44515</v>
+        <v>44514</v>
       </c>
       <c r="F4" s="4">
         <v>44528</v>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -5822,8 +5822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEC6757-7E77-4591-B8A2-6FF12E4D7889}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5862,7 +5862,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -5872,10 +5872,10 @@
       </c>
       <c r="D2" s="6">
         <f>F2-E2</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4">
-        <v>44529</v>
+        <v>44528</v>
       </c>
       <c r="F2" s="4">
         <v>44542</v>
@@ -5886,7 +5886,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -5896,10 +5896,10 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D5" si="0">F3-E3</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>44529</v>
+        <v>44528</v>
       </c>
       <c r="F3" s="4">
         <v>44542</v>
@@ -5910,7 +5910,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -5920,10 +5920,10 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4">
-        <v>44529</v>
+        <v>44528</v>
       </c>
       <c r="F4" s="4">
         <v>44542</v>
@@ -5934,7 +5934,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -5978,8 +5978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC8E347-5A34-4D73-A0FB-D96B732A0ECF}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6018,7 +6018,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -6028,10 +6028,10 @@
       </c>
       <c r="D2" s="6">
         <f>F2-E2</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
-        <v>44543</v>
+        <v>44542</v>
       </c>
       <c r="F2" s="4">
         <v>44549</v>
@@ -6042,7 +6042,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -6114,7 +6114,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>

</xml_diff>